<commit_message>
fix dictionary to show customer
</commit_message>
<xml_diff>
--- a/dictionary/dictionary.xlsx
+++ b/dictionary/dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/Desktop/R/CMML 22.07.22/dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF786303-B037-CA47-B2CE-2732D2475B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E1DC62-59DE-C543-91AA-51BB1225B9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="date" sheetId="2" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="201">
   <si>
     <t>Siem Reap</t>
   </si>
@@ -234,12 +234,6 @@
     <t>Pro Laboratory</t>
   </si>
   <si>
-    <t>Diagnostic  Detection Laboratory</t>
-  </si>
-  <si>
-    <t>Sonya Kill Memorial Hospital</t>
-  </si>
-  <si>
     <t>National Public Health Laboratory - EGASP</t>
   </si>
   <si>
@@ -672,9 +666,6 @@
     <t>NIPH -AMR project</t>
   </si>
   <si>
-    <t>NIPHL- Clean front line project</t>
-  </si>
-  <si>
     <t>NCHARDS</t>
   </si>
   <si>
@@ -697,6 +688,18 @@
   </si>
   <si>
     <t>Cammed Laboratory</t>
+  </si>
+  <si>
+    <t>Sonja Kill Memorial Hospital</t>
+  </si>
+  <si>
+    <t>Diagnostic and Detection Laboratory</t>
+  </si>
+  <si>
+    <t>NIPHL- Clean front line project</t>
+  </si>
+  <si>
+    <t>Fondation Merieux</t>
   </si>
 </sst>
 </file>
@@ -706,7 +709,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mmm/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -719,6 +722,12 @@
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -742,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -756,6 +765,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1115,15 +1128,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="5">
         <v>44562</v>
@@ -1131,7 +1144,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="5">
         <v>44926</v>
@@ -1139,7 +1152,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="5">
         <v>44562</v>
@@ -1147,7 +1160,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="5">
         <v>44926</v>
@@ -1162,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:E9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1180,7 +1193,7 @@
         <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>40</v>
@@ -1200,7 +1213,7 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D2" s="2">
         <v>103.201818</v>
@@ -1209,8 +1222,8 @@
         <v>13.108544999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
@@ -1251,7 +1264,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2">
         <v>103.201818</v>
@@ -1285,7 +1298,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="2">
         <v>104.881167</v>
@@ -1296,10 +1309,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B8" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
         <v>41</v>
@@ -1313,10 +1326,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C9" t="s">
         <v>42</v>
@@ -1348,7 +1361,7 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2">
         <v>104.906479</v>
@@ -1359,7 +1372,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>198</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -1382,7 +1395,7 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D13" s="2">
         <v>104.922798</v>
@@ -1392,14 +1405,14 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>43</v>
+      <c r="A14" s="6" t="s">
+        <v>200</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="2">
         <v>104.917811</v>
@@ -1461,7 +1474,7 @@
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
@@ -1484,7 +1497,7 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D19" s="2">
         <v>105.459999</v>
@@ -1552,7 +1565,7 @@
         <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D23" s="2">
         <v>104.89872200000001</v>
@@ -1563,13 +1576,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D24" s="2">
         <v>104.89872200000001</v>
@@ -1586,7 +1599,7 @@
         <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D25" s="2">
         <v>104.89872200000001</v>
@@ -1597,13 +1610,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D26" s="2">
         <v>104.923569</v>
@@ -1631,13 +1644,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D28" s="2">
         <v>104.89872200000001</v>
@@ -1647,14 +1660,14 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>191</v>
+      <c r="A29" s="6" t="s">
+        <v>199</v>
       </c>
       <c r="B29" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D29" s="2">
         <v>104.89872200000001</v>
@@ -1682,10 +1695,10 @@
     </row>
     <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B31" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C31" t="s">
         <v>41</v>
@@ -1739,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D34" s="2">
         <v>103.85565</v>
@@ -1767,7 +1780,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>197</v>
       </c>
       <c r="B36" t="s">
         <v>23</v>
@@ -1824,7 +1837,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D39" s="2">
         <v>104.782827</v>
@@ -1835,13 +1848,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B40" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D40" s="2">
         <v>104.906479</v>
@@ -1875,7 +1888,7 @@
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D42" s="2">
         <v>104.899123</v>
@@ -1903,7 +1916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5F89AEF-A6EC-4C4D-9139-9BBE0D706C44}">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="142" workbookViewId="0">
+    <sheetView topLeftCell="A60" zoomScale="142" workbookViewId="0">
       <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
@@ -1916,27 +1929,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
         <v>184</v>
-      </c>
-      <c r="B1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>62</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1944,13 +1957,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <v>200</v>
@@ -1958,13 +1971,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4">
         <v>1200</v>
@@ -1972,13 +1985,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -1986,13 +1999,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -2000,24 +2013,24 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
         <v>70</v>
-      </c>
-      <c r="B7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8">
         <v>1000</v>
@@ -2025,13 +2038,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9">
         <v>10000</v>
@@ -2039,13 +2052,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -2053,13 +2066,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D11">
         <v>150</v>
@@ -2067,13 +2080,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D12">
         <v>500</v>
@@ -2081,13 +2094,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D13">
         <v>500</v>
@@ -2095,13 +2108,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
         <v>79</v>
-      </c>
-      <c r="B14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" t="s">
-        <v>81</v>
       </c>
       <c r="D14">
         <v>50</v>
@@ -2109,13 +2122,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -2123,13 +2136,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D16">
         <v>8415</v>
@@ -2137,13 +2150,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D17">
         <v>7392</v>
@@ -2151,13 +2164,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D18">
         <v>10000</v>
@@ -2165,13 +2178,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D19">
         <v>100</v>
@@ -2179,13 +2192,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D20">
         <v>16000</v>
@@ -2193,13 +2206,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D21">
         <v>19000</v>
@@ -2207,13 +2220,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D22">
         <v>250</v>
@@ -2221,13 +2234,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D23">
         <v>250</v>
@@ -2235,13 +2248,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D24">
         <v>250</v>
@@ -2249,13 +2262,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D25">
         <v>50</v>
@@ -2263,13 +2276,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D26">
         <v>50</v>
@@ -2277,13 +2290,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D27">
         <v>10</v>
@@ -2291,13 +2304,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D28">
         <v>50</v>
@@ -2305,13 +2318,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D29">
         <v>5</v>
@@ -2319,13 +2332,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D30">
         <v>250</v>
@@ -2333,13 +2346,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -2347,13 +2360,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D32">
         <v>500</v>
@@ -2361,13 +2374,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D33">
         <v>50</v>
@@ -2375,13 +2388,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D34">
         <v>400</v>
@@ -2389,13 +2402,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -2403,13 +2416,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D36">
         <v>25</v>
@@ -2417,13 +2430,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D37">
         <v>50</v>
@@ -2431,13 +2444,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -2445,13 +2458,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D39">
         <v>500</v>
@@ -2459,13 +2472,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D40">
         <v>50</v>
@@ -2473,13 +2486,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C41" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D41">
         <v>10</v>
@@ -2487,24 +2500,24 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D43">
         <v>1000</v>
@@ -2512,13 +2525,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D44">
         <v>1000</v>
@@ -2526,13 +2539,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D45">
         <v>1000</v>
@@ -2540,13 +2553,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D46">
         <v>1000</v>
@@ -2554,13 +2567,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B47" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C47" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -2568,13 +2581,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D48">
         <v>3000</v>
@@ -2582,13 +2595,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B49" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D49">
         <v>24</v>
@@ -2596,13 +2609,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B50" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D50">
         <v>1500</v>
@@ -2610,13 +2623,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D51">
         <v>500</v>
@@ -2624,13 +2637,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D52">
         <v>20</v>
@@ -2638,13 +2651,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B53" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D53">
         <v>16000</v>
@@ -2652,13 +2665,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D54">
         <v>800</v>
@@ -2666,13 +2679,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D55">
         <v>20</v>
@@ -2680,13 +2693,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B56" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C56" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D56">
         <v>50</v>
@@ -2694,13 +2707,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C57" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D57">
         <v>50</v>
@@ -2708,13 +2721,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D58">
         <v>10</v>
@@ -2722,13 +2735,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D59">
         <v>500</v>
@@ -2736,13 +2749,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D60">
         <v>500</v>
@@ -2750,13 +2763,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D61">
         <v>500</v>
@@ -2764,13 +2777,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D62">
         <v>10000</v>
@@ -2778,13 +2791,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B63" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D63">
         <v>6000</v>
@@ -2792,13 +2805,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B64" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -2806,13 +2819,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D65">
         <v>200</v>
@@ -2820,13 +2833,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D66">
         <v>12000</v>
@@ -2834,13 +2847,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B67" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C67" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D67">
         <v>200</v>
@@ -2848,13 +2861,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B68" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C68" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D68">
         <v>5</v>
@@ -2862,13 +2875,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B69" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D69">
         <v>25</v>
@@ -2876,13 +2889,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C70" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D70">
         <v>100</v>
@@ -2890,24 +2903,24 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B71" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C71" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B72" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C72" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D72">
         <v>60000</v>
@@ -2915,13 +2928,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B73" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C73" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D73">
         <v>500</v>
@@ -2929,13 +2942,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B74" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C74" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D74">
         <v>200</v>
@@ -2943,13 +2956,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B75" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C75" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D75">
         <v>200</v>
@@ -2957,13 +2970,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B76" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C76" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D76">
         <v>30</v>
@@ -2971,13 +2984,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C77" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D77">
         <v>20</v>
@@ -2985,13 +2998,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B78" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C78" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D78">
         <v>120</v>
@@ -2999,35 +3012,35 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B79" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C79" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B80" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C80" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B81" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C81" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D81">
         <v>50</v>
@@ -3035,13 +3048,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B82" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C82" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D82">
         <v>50</v>
@@ -3049,13 +3062,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B83" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C83" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D83">
         <v>12000</v>
@@ -3063,13 +3076,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B84" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C84" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D84">
         <v>500</v>
@@ -3077,24 +3090,24 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B85" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C85" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B86" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C86" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D86">
         <v>500</v>
@@ -3102,13 +3115,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B87" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C87" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D87">
         <v>3500</v>
@@ -3116,24 +3129,24 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B88" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C88" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B89" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C89" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D89">
         <v>250</v>
@@ -3141,13 +3154,13 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B90" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C90" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D90">
         <v>250</v>
@@ -3155,24 +3168,24 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B91" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C91" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B92" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C92" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D92">
         <v>9</v>
@@ -3180,13 +3193,13 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B93" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C93" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D93">
         <v>100</v>
@@ -3194,13 +3207,13 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B94" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C94" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D94">
         <v>200</v>
@@ -3208,13 +3221,13 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B95" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C95" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D95">
         <v>960</v>
@@ -3222,13 +3235,13 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B96" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C96" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D96">
         <v>200</v>
@@ -3236,13 +3249,13 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B97" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C97" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D97">
         <v>500</v>
@@ -3250,13 +3263,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B98" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C98" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D98">
         <v>5</v>
@@ -3264,13 +3277,13 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B99" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C99" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D99">
         <v>200</v>
@@ -3278,13 +3291,13 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B100" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C100" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D100">
         <v>200</v>
@@ -3292,13 +3305,13 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B101" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C101" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D101">
         <v>20</v>
@@ -3306,13 +3319,13 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B102" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C102" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D102">
         <v>200</v>
@@ -3320,13 +3333,13 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B103" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C103" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D103">
         <v>1500</v>
@@ -3334,13 +3347,13 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B104" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C104" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D104">
         <v>50</v>
@@ -3348,24 +3361,24 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B105" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C105" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B106" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C106" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D106">
         <v>13000</v>
@@ -3373,13 +3386,13 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B107" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C107" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D107">
         <v>200</v>
@@ -3387,13 +3400,13 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B108" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C108" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D108">
         <v>960</v>
@@ -3401,13 +3414,13 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B109" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C109" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D109">
         <v>250</v>
@@ -3415,13 +3428,13 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B110" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C110" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D110">
         <v>400</v>
@@ -3429,13 +3442,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B111" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C111" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D111">
         <v>50</v>
@@ -3443,13 +3456,13 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B112" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C112" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D112">
         <v>3000</v>
@@ -3457,24 +3470,24 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B113" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C113" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B114" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C114" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
matching customer with lowercase
</commit_message>
<xml_diff>
--- a/dictionary/dictionary.xlsx
+++ b/dictionary/dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/Desktop/R/CMML 22.07.22/dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E1DC62-59DE-C543-91AA-51BB1225B9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEAF021-C23F-C84E-99D9-23FB07D902C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1175,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>